<commit_message>
Proof read all docs and attached completed Gantt
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Atticus\Desktop\2810ICT Soft Tech\Ass A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Atticus\Desktop\2810ICT Soft Tech\Repo\Assignment-Software-Technologies-Group31\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6C78E6-1E89-4B09-81F6-2E738EA4F9A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4E6A90-9137-4D3F-9E8C-838CFDAD635A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,10 +189,10 @@
     <t>3.4 User Interface</t>
   </si>
   <si>
-    <t>Days</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Day Highlight:</t>
+  </si>
+  <si>
+    <t>Days. Started on 7.8.23</t>
   </si>
 </sst>
 </file>
@@ -572,77 +572,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="7" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="8" borderId="8" xfId="6" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="7" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="9" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="8" borderId="8" xfId="6" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1047,7 +1047,7 @@
   <dimension ref="B1:BO17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+      <selection activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1074,51 +1074,51 @@
       <c r="G1" s="8"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="30" t="s">
-        <v>27</v>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="19" t="s">
+        <v>26</v>
       </c>
       <c r="H2" s="10">
         <v>1</v>
       </c>
       <c r="J2" s="11"/>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="22"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="33"/>
       <c r="P2" s="12"/>
-      <c r="Q2" s="20" t="s">
+      <c r="Q2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="22"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="33"/>
       <c r="U2" s="13"/>
-      <c r="V2" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="26"/>
+      <c r="V2" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="37"/>
       <c r="Z2" s="14"/>
-      <c r="AA2" s="27" t="s">
+      <c r="AA2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="28"/>
-      <c r="AC2" s="28"/>
-      <c r="AD2" s="28"/>
-      <c r="AE2" s="28"/>
-      <c r="AF2" s="28"/>
-      <c r="AG2" s="29"/>
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39"/>
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
+      <c r="AG2" s="40"/>
       <c r="AH2" s="15"/>
       <c r="AI2" s="17" t="s">
         <v>3</v>
@@ -1132,26 +1132,26 @@
       <c r="AP2" s="18"/>
     </row>
     <row r="3" spans="2:67" s="7" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="30" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="6"/>
@@ -1174,12 +1174,12 @@
       <c r="AA3" s="6"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1362,236 +1362,278 @@
       </c>
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="42">
-        <v>1</v>
-      </c>
-      <c r="D5" s="42">
-        <v>5</v>
-      </c>
-      <c r="E5" s="42">
+      <c r="C5" s="29">
+        <v>1</v>
+      </c>
+      <c r="D5" s="29">
+        <v>4</v>
+      </c>
+      <c r="E5" s="29">
         <v>3</v>
       </c>
-      <c r="F5" s="42">
-        <v>5</v>
-      </c>
-      <c r="G5" s="39">
+      <c r="F5" s="29">
+        <v>3</v>
+      </c>
+      <c r="G5" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="34">
-        <v>1</v>
-      </c>
-      <c r="D6" s="34">
-        <v>2</v>
-      </c>
-      <c r="E6" s="34">
-        <v>2</v>
-      </c>
-      <c r="F6" s="34">
+      <c r="C6" s="21">
+        <v>1</v>
+      </c>
+      <c r="D6" s="21">
+        <v>1</v>
+      </c>
+      <c r="E6" s="21">
+        <v>1</v>
+      </c>
+      <c r="F6" s="21">
         <v>3</v>
       </c>
-      <c r="G6" s="35">
+      <c r="G6" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="34">
-        <v>1</v>
-      </c>
-      <c r="D7" s="34">
-        <v>3</v>
-      </c>
-      <c r="E7" s="34">
-        <v>4</v>
-      </c>
-      <c r="F7" s="34">
-        <v>2</v>
-      </c>
-      <c r="G7" s="35">
+      <c r="C7" s="21">
+        <v>1</v>
+      </c>
+      <c r="D7" s="21">
+        <v>1</v>
+      </c>
+      <c r="E7" s="21">
+        <v>1</v>
+      </c>
+      <c r="F7" s="21">
+        <v>1</v>
+      </c>
+      <c r="G7" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="34">
-        <v>1</v>
-      </c>
-      <c r="D8" s="34">
+      <c r="C8" s="21">
+        <v>1</v>
+      </c>
+      <c r="D8" s="21">
         <v>4</v>
       </c>
-      <c r="E8" s="34">
-        <v>3</v>
-      </c>
-      <c r="F8" s="34">
-        <v>5</v>
-      </c>
-      <c r="G8" s="35">
+      <c r="E8" s="21">
+        <v>2</v>
+      </c>
+      <c r="F8" s="21">
+        <v>4</v>
+      </c>
+      <c r="G8" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="38">
-        <v>8</v>
-      </c>
-      <c r="D9" s="38">
-        <v>9</v>
-      </c>
-      <c r="E9" s="38">
-        <v>8</v>
-      </c>
-      <c r="F9" s="38">
-        <v>10</v>
-      </c>
-      <c r="G9" s="39">
-        <v>0.9</v>
+      <c r="C9" s="25">
+        <v>5</v>
+      </c>
+      <c r="D9" s="25">
+        <v>5</v>
+      </c>
+      <c r="E9" s="25">
+        <v>6</v>
+      </c>
+      <c r="F9" s="25">
+        <v>5</v>
+      </c>
+      <c r="G9" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="34">
-        <v>8</v>
-      </c>
-      <c r="D10" s="34">
-        <v>3</v>
-      </c>
-      <c r="E10" s="34">
-        <v>9</v>
-      </c>
-      <c r="F10" s="34">
-        <v>2</v>
-      </c>
-      <c r="G10" s="35">
+      <c r="C10" s="21">
+        <v>5</v>
+      </c>
+      <c r="D10" s="21">
+        <v>1</v>
+      </c>
+      <c r="E10" s="21">
+        <v>5</v>
+      </c>
+      <c r="F10" s="21">
+        <v>1</v>
+      </c>
+      <c r="G10" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="34">
-        <v>9</v>
-      </c>
-      <c r="D11" s="34">
-        <v>8</v>
-      </c>
-      <c r="E11" s="34">
-        <v>9</v>
-      </c>
-      <c r="F11" s="34">
+      <c r="C11" s="21">
+        <v>5</v>
+      </c>
+      <c r="D11" s="21">
+        <v>4</v>
+      </c>
+      <c r="E11" s="21">
         <v>6</v>
       </c>
-      <c r="G11" s="35">
+      <c r="F11" s="21">
+        <v>4</v>
+      </c>
+      <c r="G11" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="34">
-        <v>9</v>
-      </c>
-      <c r="D12" s="34">
-        <v>10</v>
-      </c>
-      <c r="E12" s="34">
-        <v>9</v>
-      </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="35">
-        <v>0</v>
+      <c r="C12" s="21">
+        <v>3</v>
+      </c>
+      <c r="D12" s="21">
+        <v>15</v>
+      </c>
+      <c r="E12" s="21">
+        <v>4</v>
+      </c>
+      <c r="F12" s="21">
+        <v>14</v>
+      </c>
+      <c r="G12" s="22">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="39">
-        <v>0</v>
+      <c r="C13" s="25">
+        <v>12</v>
+      </c>
+      <c r="D13" s="25">
+        <v>4</v>
+      </c>
+      <c r="E13" s="25">
+        <v>13</v>
+      </c>
+      <c r="F13" s="25">
+        <v>5</v>
+      </c>
+      <c r="G13" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="35">
-        <v>0</v>
+      <c r="C14" s="21">
+        <v>12</v>
+      </c>
+      <c r="D14" s="21">
+        <v>3</v>
+      </c>
+      <c r="E14" s="21">
+        <v>13</v>
+      </c>
+      <c r="F14" s="21">
+        <v>4</v>
+      </c>
+      <c r="G14" s="22">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="35">
-        <v>0</v>
+      <c r="C15" s="23">
+        <v>12</v>
+      </c>
+      <c r="D15" s="21">
+        <v>3</v>
+      </c>
+      <c r="E15" s="21">
+        <v>13</v>
+      </c>
+      <c r="F15" s="21">
+        <v>4</v>
+      </c>
+      <c r="G15" s="22">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="35">
-        <v>0</v>
+      <c r="C16" s="21">
+        <v>13</v>
+      </c>
+      <c r="D16" s="21">
+        <v>3</v>
+      </c>
+      <c r="E16" s="21">
+        <v>13</v>
+      </c>
+      <c r="F16" s="21">
+        <v>4</v>
+      </c>
+      <c r="G16" s="22">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="35">
-        <v>0</v>
+      <c r="C17" s="21">
+        <v>13</v>
+      </c>
+      <c r="D17" s="21">
+        <v>4</v>
+      </c>
+      <c r="E17" s="21">
+        <v>13</v>
+      </c>
+      <c r="F17" s="21">
+        <v>5</v>
+      </c>
+      <c r="G17" s="22">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:BO17">
     <cfRule type="expression" dxfId="8" priority="1">

</xml_diff>